<commit_message>
test xml and parameterization from xml added
</commit_message>
<xml_diff>
--- a/test-data/orange_data.xlsx
+++ b/test-data/orange_data.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9804" windowHeight="3264"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9804" windowHeight="3264" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="validCredentialTest" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -378,7 +378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -433,7 +433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
connected excel for valid credential test
</commit_message>
<xml_diff>
--- a/test-data/orange_data.xlsx
+++ b/test-data/orange_data.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9804" windowHeight="3264" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9804" windowHeight="3264" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="1" r:id="rId1"/>
-    <sheet name="validCredentialTest" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="validCredentialTest" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -51,6 +50,18 @@
   </si>
   <si>
     <t>wick123</t>
+  </si>
+  <si>
+    <t>Expected Value</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Employee List</t>
   </si>
 </sst>
 </file>
@@ -431,14 +442,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -453,16 +501,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>